<commit_message>
Last touches on report and presentation
</commit_message>
<xml_diff>
--- a/MEng_TaskB/Data analysis and modelling/classification_model_results.xlsx
+++ b/MEng_TaskB/Data analysis and modelling/classification_model_results.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isabel/SUN/03_DataScience/00_PostBlock/PBA3_19May/ds-group-42-pba-3/MEng_TaskB/Adult/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isabel/SUN/03_DataScience/00_PostBlock/PBA3_19May/ds-group-42-pba-3/MEng_TaskB/Data analysis and modelling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA63CF82-E722-4B4A-BEAB-C0E347C0A9C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA1B5067-1D38-C349-B12D-D1C3D655EA1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24754,9 +24754,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
+      <xdr:colOff>222250</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>28222</xdr:rowOff>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -24824,15 +24824,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
+      <xdr:colOff>338666</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>152399</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>736600</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>155222</xdr:rowOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>74082</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -26867,16 +26867,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A25:I25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="H26:I26"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A25:I25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="H26:I26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -27750,8 +27750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FF06522-7AD8-8F4F-B195-C56521A4F0C4}">
   <dimension ref="A1:X34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J20" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="AB38" sqref="AB38"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="R29" sqref="R29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
worked on some stuff
</commit_message>
<xml_diff>
--- a/MEng_TaskB/Data analysis and modelling/classification_model_results.xlsx
+++ b/MEng_TaskB/Data analysis and modelling/classification_model_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isabel/SUN/03_DataScience/00_PostBlock/PBA3_19May/ds-group-42-pba-3/MEng_TaskB/Data analysis and modelling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA1B5067-1D38-C349-B12D-D1C3D655EA1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{710DABF2-F748-944A-A5CF-5D518B3ED0F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7512,201 +7512,8 @@
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="3"/>
+          <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'NewResults_End)'!$B$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Control(Accuracy)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent5">
-                <a:lumMod val="50000"/>
-              </a:schemeClr>
-            </a:solidFill>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:numRef>
-              <c:f>'NewResults_End)'!$A$4:$A$6</c:f>
-              <c:numCache>
-                <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>0.1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.7</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'NewResults_End)'!$B$4:$B$6</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>0.81113727095915655</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.81113727095915655</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.81113727095915655</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000009-6F6E-5449-AFCC-88C437AA697E}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'NewResults_End)'!$C$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Mean(Accuracy)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent5">
-                <a:lumMod val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:numRef>
-              <c:f>'NewResults_End)'!$A$4:$A$6</c:f>
-              <c:numCache>
-                <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>0.1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.7</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'NewResults_End)'!$C$4:$C$6</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>0.8123656464325929</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.78104207185996521</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.76292353362677856</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000A-6F6E-5449-AFCC-88C437AA697E}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'NewResults_End)'!$D$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>k-NN(Accuracy)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent5">
-                <a:lumMod val="60000"/>
-                <a:lumOff val="40000"/>
-              </a:schemeClr>
-            </a:solidFill>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:numRef>
-              <c:f>'NewResults_End)'!$A$4:$A$6</c:f>
-              <c:numCache>
-                <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>0.1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.7</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'NewResults_End)'!$D$4:$D$6</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>0.80663300000000004</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.56658799999999998</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.26164399999999999</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000B-6F6E-5449-AFCC-88C437AA697E}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="3"/>
           <c:tx>
             <c:strRef>
               <c:f>'NewResults_End)'!$N$3</c:f>
@@ -7774,7 +7581,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="4"/>
+          <c:order val="1"/>
           <c:tx>
             <c:strRef>
               <c:f>'NewResults_End)'!$O$3</c:f>
@@ -7843,7 +7650,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="5"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
               <c:f>'NewResults_End)'!$P$3</c:f>
@@ -8138,201 +7945,8 @@
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="3"/>
+          <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'NewResults_End)'!$B$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Control(Accuracy)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent5">
-                <a:lumMod val="50000"/>
-              </a:schemeClr>
-            </a:solidFill>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:numRef>
-              <c:f>'NewResults_End)'!$A$27:$A$29</c:f>
-              <c:numCache>
-                <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>0.1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.7</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'NewResults_End)'!$B$27:$B$29</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>0.80745214453884695</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.80745214453884695</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.80745214453884695</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000009-AB5A-AD40-BE72-FB4A83BC126D}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'NewResults_End)'!$C$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Mean(Accuracy)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent5">
-                <a:lumMod val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:numRef>
-              <c:f>'NewResults_End)'!$A$27:$A$29</c:f>
-              <c:numCache>
-                <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>0.1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.7</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'NewResults_End)'!$C$27:$C$29</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>0.78513665677141975</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.77459310062442421</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.74961613266455118</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000A-AB5A-AD40-BE72-FB4A83BC126D}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'NewResults_End)'!$D$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>k-NN(Accuracy)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent5">
-                <a:lumMod val="60000"/>
-                <a:lumOff val="40000"/>
-              </a:schemeClr>
-            </a:solidFill>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:numRef>
-              <c:f>'NewResults_End)'!$A$27:$A$29</c:f>
-              <c:numCache>
-                <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>0.1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.7</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'NewResults_End)'!$D$27:$D$29</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>0.78431799999999996</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.61203799999999997</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.31958199999999998</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000B-AB5A-AD40-BE72-FB4A83BC126D}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="3"/>
           <c:tx>
             <c:strRef>
               <c:f>'NewResults_End)'!$N$3</c:f>
@@ -8400,7 +8014,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="4"/>
+          <c:order val="1"/>
           <c:tx>
             <c:strRef>
               <c:f>'NewResults_End)'!$O$3</c:f>
@@ -8469,7 +8083,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="5"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
               <c:f>'NewResults_End)'!$P$3</c:f>
@@ -8734,7 +8348,7 @@
       </c:valAx>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
+      <c:legendPos val="b"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -26867,16 +26481,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="A1:I1"/>
     <mergeCell ref="A25:I25"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="D26:E26"/>
     <mergeCell ref="F26:G26"/>
     <mergeCell ref="H26:I26"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="A1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -27750,8 +27364,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FF06522-7AD8-8F4F-B195-C56521A4F0C4}">
   <dimension ref="A1:X34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="R29" sqref="R29"/>
+    <sheetView tabSelected="1" topLeftCell="J14" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="AC42" sqref="AC42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>